<commit_message>
menambahkan fitur kelas perkuliahan
</commit_message>
<xml_diff>
--- a/template/kelas_template.xlsx
+++ b/template/kelas_template.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\wsclient-new\template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20055" windowHeight="7935" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20055" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="kelas" sheetId="1" r:id="rId1"/>
@@ -18,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="43">
   <si>
     <t>Nama Mahasiswa</t>
   </si>
@@ -89,18 +94,6 @@
     <t>Kelas Perkuliahan</t>
   </si>
   <si>
-    <t>Kode Prodi</t>
-  </si>
-  <si>
-    <t>Program Studi</t>
-  </si>
-  <si>
-    <t>Kode Program Studi</t>
-  </si>
-  <si>
-    <t>Nama Program Studi</t>
-  </si>
-  <si>
     <t>Mahasiswa</t>
   </si>
   <si>
@@ -149,17 +142,26 @@
     <t>- Tabel Nilai</t>
   </si>
   <si>
-    <t>Nama Program Studi (Opsional)</t>
+    <t>Id_sms</t>
+  </si>
+  <si>
+    <t>Jenjang_pendidikan</t>
+  </si>
+  <si>
+    <t>Jangan diganti. Merupakan kode Prodi</t>
+  </si>
+  <si>
+    <t>Jangan diganti. Jejang Pendidikan Pada prodi tersebut</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,7 +305,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -486,6 +488,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -732,7 +740,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -797,6 +805,9 @@
     <xf numFmtId="0" fontId="16" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="34" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -845,6 +856,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -891,7 +910,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -923,9 +942,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -957,6 +977,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1132,17 +1153,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" style="1" customWidth="1"/>
@@ -1154,7 +1175,7 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33" customHeight="1">
+    <row r="1" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
@@ -1171,13 +1192,13 @@
         <v>21</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="20.25" customHeight="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1193,17 +1214,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H1" sqref="H1:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" style="1" customWidth="1"/>
@@ -1216,7 +1237,7 @@
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="33" customHeight="1">
+    <row r="1" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
@@ -1224,13 +1245,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>21</v>
@@ -1239,13 +1260,13 @@
         <v>3</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="20.25" customHeight="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1263,17 +1284,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="J1" sqref="J1:K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" style="1" customWidth="1"/>
@@ -1288,42 +1309,42 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="33" customHeight="1">
+    <row r="1" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>21</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>3</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="20.25" customHeight="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1343,17 +1364,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:L1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" style="1" customWidth="1"/>
@@ -1368,7 +1389,7 @@
     <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="33" customHeight="1">
+    <row r="1" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
@@ -1400,13 +1421,13 @@
         <v>12</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="20.25" customHeight="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1427,17 +1448,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
@@ -1445,7 +1466,7 @@
     <col min="7" max="7" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="27" customHeight="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
@@ -1456,10 +1477,10 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="27" customHeight="1">
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="20" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1467,7 +1488,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="27.75" customHeight="1">
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1482,7 +1503,7 @@
       <c r="F3" s="22"/>
       <c r="G3" s="23"/>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -1497,7 +1518,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -1512,7 +1533,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -1527,7 +1548,7 @@
       <c r="F6" s="4"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -1542,40 +1563,40 @@
       <c r="F7" s="4"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" ht="21" customHeight="1">
+    <row r="8" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>10</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>23</v>
+      <c r="B8" s="24" t="s">
+        <v>39</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="18"/>
     </row>
-    <row r="9" spans="1:7" ht="21" customHeight="1">
+    <row r="9" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>11</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>24</v>
+      <c r="B9" s="24" t="s">
+        <v>40</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="18"/>
     </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" ht="27" customHeight="1">
+    <row r="12" spans="1:7" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="20" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1583,7 +1604,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" ht="27.75" customHeight="1">
+    <row r="13" spans="1:7" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>6</v>
       </c>
@@ -1598,7 +1619,7 @@
       <c r="F13" s="22"/>
       <c r="G13" s="23"/>
     </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1">
+    <row r="14" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>1</v>
       </c>
@@ -1613,7 +1634,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="15" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>2</v>
       </c>
@@ -1628,7 +1649,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="16" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>3</v>
       </c>
@@ -1643,7 +1664,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="17" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>4</v>
       </c>
@@ -1658,7 +1679,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="18" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>5</v>
       </c>
@@ -1673,7 +1694,7 @@
       <c r="F18" s="4"/>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="19" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>6</v>
       </c>
@@ -1688,40 +1709,40 @@
       <c r="F19" s="4"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7" ht="21" customHeight="1">
+    <row r="20" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>7</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>23</v>
+      <c r="B20" s="24" t="s">
+        <v>39</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="18"/>
     </row>
-    <row r="21" spans="1:7" ht="21" customHeight="1">
+    <row r="21" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>8</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>24</v>
+      <c r="B21" s="24" t="s">
+        <v>40</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" s="14"/>
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
       <c r="G21" s="18"/>
     </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" ht="27" customHeight="1">
+    <row r="24" spans="1:7" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="20" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1729,7 +1750,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" s="1" customFormat="1" ht="27.75" customHeight="1">
+    <row r="25" spans="1:7" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>6</v>
       </c>
@@ -1744,37 +1765,37 @@
       <c r="F25" s="22"/>
       <c r="G25" s="23"/>
     </row>
-    <row r="26" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1">
+    <row r="26" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>1</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="27" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>2</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="28" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>3</v>
       </c>
@@ -1789,7 +1810,7 @@
       <c r="F28" s="4"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="29" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>4</v>
       </c>
@@ -1804,37 +1825,37 @@
       <c r="F29" s="4"/>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="30" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>5</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="31" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>6</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="32" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>7</v>
       </c>
@@ -1849,41 +1870,41 @@
       <c r="F32" s="4"/>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="1:7" ht="21" customHeight="1">
+    <row r="33" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>8</v>
       </c>
-      <c r="B33" s="13" t="s">
-        <v>23</v>
+      <c r="B33" s="24" t="s">
+        <v>39</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="D33" s="14"/>
       <c r="E33" s="17"/>
       <c r="F33" s="17"/>
       <c r="G33" s="18"/>
     </row>
-    <row r="34" spans="1:7" ht="21" customHeight="1">
+    <row r="34" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>9</v>
       </c>
-      <c r="B34" s="13" t="s">
-        <v>24</v>
+      <c r="B34" s="24" t="s">
+        <v>40</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D34" s="14"/>
       <c r="E34" s="17"/>
       <c r="F34" s="17"/>
       <c r="G34" s="18"/>
     </row>
-    <row r="35" spans="1:7" ht="13.5" customHeight="1"/>
-    <row r="37" spans="1:7" s="1" customFormat="1" ht="27" customHeight="1">
+    <row r="35" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:7" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="20" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -1891,7 +1912,7 @@
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="1:7" s="1" customFormat="1" ht="27.75" customHeight="1">
+    <row r="38" spans="1:7" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>6</v>
       </c>
@@ -1906,7 +1927,7 @@
       <c r="F38" s="22"/>
       <c r="G38" s="23"/>
     </row>
-    <row r="39" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1">
+    <row r="39" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>1</v>
       </c>
@@ -1921,7 +1942,7 @@
       <c r="F39" s="4"/>
       <c r="G39" s="5"/>
     </row>
-    <row r="40" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="40" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>2</v>
       </c>
@@ -1936,7 +1957,7 @@
       <c r="F40" s="4"/>
       <c r="G40" s="5"/>
     </row>
-    <row r="41" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="41" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <v>3</v>
       </c>
@@ -1951,7 +1972,7 @@
       <c r="F41" s="4"/>
       <c r="G41" s="5"/>
     </row>
-    <row r="42" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="42" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>4</v>
       </c>
@@ -1966,7 +1987,7 @@
       <c r="F42" s="4"/>
       <c r="G42" s="5"/>
     </row>
-    <row r="43" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="43" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <v>5</v>
       </c>
@@ -1981,7 +2002,7 @@
       <c r="F43" s="4"/>
       <c r="G43" s="5"/>
     </row>
-    <row r="44" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="44" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="9">
         <v>6</v>
       </c>
@@ -1996,7 +2017,7 @@
       <c r="F44" s="4"/>
       <c r="G44" s="5"/>
     </row>
-    <row r="45" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="45" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
         <v>7</v>
       </c>
@@ -2011,7 +2032,7 @@
       <c r="F45" s="4"/>
       <c r="G45" s="5"/>
     </row>
-    <row r="46" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="46" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
         <v>8</v>
       </c>
@@ -2026,7 +2047,7 @@
       <c r="F46" s="4"/>
       <c r="G46" s="5"/>
     </row>
-    <row r="47" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="47" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
         <v>9</v>
       </c>
@@ -2041,30 +2062,30 @@
       <c r="F47" s="15"/>
       <c r="G47" s="16"/>
     </row>
-    <row r="48" spans="1:7" ht="21" customHeight="1">
+    <row r="48" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
         <v>10</v>
       </c>
-      <c r="B48" s="13" t="s">
-        <v>23</v>
+      <c r="B48" s="24" t="s">
+        <v>39</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="D48" s="14"/>
       <c r="E48" s="17"/>
       <c r="F48" s="17"/>
       <c r="G48" s="18"/>
     </row>
-    <row r="49" spans="1:7" ht="21" customHeight="1">
+    <row r="49" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12">
         <v>11</v>
       </c>
-      <c r="B49" s="13" t="s">
-        <v>24</v>
+      <c r="B49" s="24" t="s">
+        <v>40</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="D49" s="14"/>
       <c r="E49" s="17"/>

</xml_diff>